<commit_message>
New New York it203
</commit_message>
<xml_diff>
--- a/NewYork/it203-current.xlsx
+++ b/NewYork/it203-current.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JCC\ewc\taxes\tax_worksheets\NewYork\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ewc\tax_worksheets\NewYork\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="165">
   <si>
     <t>IT-203 - Nonresident and Part-Year Resident Income Tax Return</t>
   </si>
@@ -581,6 +581,12 @@
       </rPr>
       <t xml:space="preserve"> (add lines 60 through 65)</t>
     </r>
+  </si>
+  <si>
+    <t>60a</t>
+  </si>
+  <si>
+    <t>NYC school tax credit (rate reduction amount)</t>
   </si>
 </sst>
 </file>
@@ -636,13 +642,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor theme="0"/>
         <bgColor indexed="26"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FFFFFF99"/>
         <bgColor indexed="26"/>
       </patternFill>
     </fill>
@@ -888,8 +894,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -915,9 +919,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="18" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -992,6 +998,9 @@
       <rgbColor rgb="004A3285"/>
       <rgbColor rgb="00424242"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FFFFFF99"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1267,7 +1276,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F85"/>
+  <dimension ref="A1:F86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="142" workbookViewId="0"/>
   </sheetViews>
@@ -1307,14 +1316,14 @@
       <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="15" t="s">
+      <c r="D4" s="14"/>
+      <c r="E4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="16"/>
+      <c r="F4" s="14"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="6" t="s">
@@ -1323,14 +1332,14 @@
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="15" t="s">
+      <c r="D5" s="14"/>
+      <c r="E5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="16"/>
+      <c r="F5" s="14"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="6" t="s">
@@ -1339,14 +1348,14 @@
       <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="15" t="s">
+      <c r="D6" s="14"/>
+      <c r="E6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="16"/>
+      <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="6" t="s">
@@ -1355,14 +1364,14 @@
       <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="15" t="s">
+      <c r="D7" s="14"/>
+      <c r="E7" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="16"/>
+      <c r="F7" s="14"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="6" t="s">
@@ -1371,14 +1380,14 @@
       <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="15" t="s">
+      <c r="D8" s="14"/>
+      <c r="E8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="16"/>
+      <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="6" t="s">
@@ -1387,14 +1396,14 @@
       <c r="B9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="15" t="s">
+      <c r="D9" s="14"/>
+      <c r="E9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="16"/>
+      <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="6" t="s">
@@ -1403,14 +1412,14 @@
       <c r="B10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="15" t="s">
+      <c r="D10" s="14"/>
+      <c r="E10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="16"/>
+      <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="6" t="s">
@@ -1419,14 +1428,14 @@
       <c r="B11" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="15" t="s">
+      <c r="D11" s="14"/>
+      <c r="E11" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="16"/>
+      <c r="F11" s="14"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="6" t="s">
@@ -1435,14 +1444,14 @@
       <c r="B12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="15" t="s">
+      <c r="D12" s="14"/>
+      <c r="E12" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="16"/>
+      <c r="F12" s="14"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="6" t="s">
@@ -1451,14 +1460,14 @@
       <c r="B13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="15" t="s">
+      <c r="D13" s="14"/>
+      <c r="E13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="16"/>
+      <c r="F13" s="14"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="6" t="s">
@@ -1467,14 +1476,14 @@
       <c r="B14" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="15" t="s">
+      <c r="D14" s="14"/>
+      <c r="E14" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="16"/>
+      <c r="F14" s="14"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="6" t="s">
@@ -1483,12 +1492,12 @@
       <c r="B15" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="24"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="22"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="6" t="s">
@@ -1497,14 +1506,14 @@
       <c r="B16" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="15" t="s">
+      <c r="D16" s="14"/>
+      <c r="E16" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="F16" s="16"/>
+      <c r="F16" s="14"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="6" t="s">
@@ -1513,30 +1522,30 @@
       <c r="B17" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="16"/>
-      <c r="E17" s="15" t="s">
+      <c r="D17" s="14"/>
+      <c r="E17" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="16"/>
+      <c r="F17" s="14"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="15" t="s">
+      <c r="D18" s="14"/>
+      <c r="E18" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="16"/>
+      <c r="F18" s="14"/>
     </row>
     <row r="19" spans="1:6" ht="13.5" thickBot="1">
       <c r="A19" s="6" t="s">
@@ -1545,14 +1554,14 @@
       <c r="B19" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="22"/>
-      <c r="E19" s="21" t="s">
+      <c r="D19" s="20"/>
+      <c r="E19" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="22"/>
+      <c r="F19" s="20"/>
     </row>
     <row r="20" spans="1:6" ht="13.5" thickTop="1">
       <c r="A20" s="6" t="s">
@@ -1561,17 +1570,17 @@
       <c r="B20" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="25">
+      <c r="D20" s="23">
         <f>SUM(D4:D14)+SUM(D16:D19)</f>
         <v>0</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="F20" s="20">
+      <c r="F20" s="18">
         <f>SUM(F4:F14)+SUM(F16:F19)</f>
         <v>0</v>
       </c>
@@ -1583,14 +1592,14 @@
       <c r="B21" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="26"/>
-      <c r="E21" s="21" t="s">
+      <c r="D21" s="24"/>
+      <c r="E21" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="F21" s="22"/>
+      <c r="F21" s="20"/>
     </row>
     <row r="22" spans="1:6" ht="13.5" thickTop="1">
       <c r="A22" s="6" t="s">
@@ -1599,39 +1608,39 @@
       <c r="B22" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="25">
+      <c r="D22" s="23">
         <f>D20-D21</f>
         <v>0</v>
       </c>
-      <c r="E22" s="19" t="s">
+      <c r="E22" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="F22" s="20">
+      <c r="F22" s="18">
         <f>F20-F21</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="D23" s="27">
+      <c r="D23" s="25">
         <f>D22</f>
         <v>0</v>
       </c>
-      <c r="E23" s="17" t="s">
+      <c r="E23" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="F23" s="18">
+      <c r="F23" s="16">
         <f>F22</f>
         <v>0</v>
       </c>
@@ -1643,14 +1652,14 @@
       <c r="B24" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C24" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="28"/>
-      <c r="E24" s="15" t="s">
+      <c r="D24" s="26"/>
+      <c r="E24" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F24" s="16"/>
+      <c r="F24" s="14"/>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="6" t="s">
@@ -1659,14 +1668,14 @@
       <c r="B25" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="28"/>
-      <c r="E25" s="15" t="s">
+      <c r="D25" s="26"/>
+      <c r="E25" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="F25" s="16"/>
+      <c r="F25" s="14"/>
     </row>
     <row r="26" spans="1:6" ht="13.5" thickBot="1">
       <c r="A26" s="6" t="s">
@@ -1675,14 +1684,14 @@
       <c r="B26" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="D26" s="26"/>
-      <c r="E26" s="21" t="s">
+      <c r="D26" s="24"/>
+      <c r="E26" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="F26" s="22"/>
+      <c r="F26" s="20"/>
     </row>
     <row r="27" spans="1:6" ht="13.5" thickTop="1">
       <c r="A27" s="6" t="s">
@@ -1691,17 +1700,17 @@
       <c r="B27" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="C27" s="19" t="s">
+      <c r="C27" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D27" s="25">
+      <c r="D27" s="23">
         <f>SUM(D23:D26)</f>
         <v>0</v>
       </c>
-      <c r="E27" s="19" t="s">
+      <c r="E27" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="F27" s="20">
+      <c r="F27" s="18">
         <f>SUM(F23:F26)</f>
         <v>0</v>
       </c>
@@ -1713,17 +1722,17 @@
       <c r="B28" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D28" s="28">
+      <c r="D28" s="26">
         <f>D7</f>
         <v>0</v>
       </c>
-      <c r="E28" s="15" t="s">
+      <c r="E28" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="F28" s="16">
+      <c r="F28" s="14">
         <f>F7</f>
         <v>0</v>
       </c>
@@ -1735,14 +1744,14 @@
       <c r="B29" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="15" t="s">
+      <c r="C29" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="28"/>
-      <c r="E29" s="15" t="s">
+      <c r="D29" s="26"/>
+      <c r="E29" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="F29" s="16"/>
+      <c r="F29" s="14"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="6" t="s">
@@ -1751,14 +1760,14 @@
       <c r="B30" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D30" s="28"/>
-      <c r="E30" s="15" t="s">
+      <c r="D30" s="26"/>
+      <c r="E30" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F30" s="16"/>
+      <c r="F30" s="14"/>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="6" t="s">
@@ -1767,14 +1776,14 @@
       <c r="B31" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="28"/>
-      <c r="E31" s="15" t="s">
+      <c r="D31" s="26"/>
+      <c r="E31" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="F31" s="16"/>
+      <c r="F31" s="14"/>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="6" t="s">
@@ -1783,14 +1792,14 @@
       <c r="B32" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="C32" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D32" s="28"/>
-      <c r="E32" s="15" t="s">
+      <c r="D32" s="26"/>
+      <c r="E32" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="F32" s="16"/>
+      <c r="F32" s="14"/>
     </row>
     <row r="33" spans="1:6" ht="13.5" thickBot="1">
       <c r="A33" s="6" t="s">
@@ -1799,14 +1808,14 @@
       <c r="B33" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C33" s="21" t="s">
+      <c r="C33" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="D33" s="26"/>
-      <c r="E33" s="21" t="s">
+      <c r="D33" s="24"/>
+      <c r="E33" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="F33" s="22"/>
+      <c r="F33" s="20"/>
     </row>
     <row r="34" spans="1:6" ht="14.25" thickTop="1" thickBot="1">
       <c r="A34" s="6" t="s">
@@ -1815,17 +1824,17 @@
       <c r="B34" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C34" s="29" t="s">
+      <c r="C34" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="D34" s="30">
+      <c r="D34" s="28">
         <f>SUM(D28:D33)</f>
         <v>0</v>
       </c>
-      <c r="E34" s="29" t="s">
+      <c r="E34" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="F34" s="31">
+      <c r="F34" s="29">
         <f>SUM(F28:F33)</f>
         <v>0</v>
       </c>
@@ -1837,17 +1846,17 @@
       <c r="B35" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="19" t="s">
+      <c r="C35" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D35" s="25">
+      <c r="D35" s="23">
         <f>D27-D34</f>
         <v>0</v>
       </c>
-      <c r="E35" s="19" t="s">
+      <c r="E35" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="F35" s="20">
+      <c r="F35" s="18">
         <f>F27-F34</f>
         <v>0</v>
       </c>
@@ -1861,10 +1870,10 @@
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
-      <c r="E36" s="15" t="s">
+      <c r="E36" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="F36" s="16">
+      <c r="F36" s="14">
         <f>D35</f>
         <v>0</v>
       </c>
@@ -1878,10 +1887,10 @@
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
-      <c r="E37" s="21" t="s">
+      <c r="E37" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="F37" s="22"/>
+      <c r="F37" s="20"/>
     </row>
     <row r="38" spans="1:6" ht="13.5" thickTop="1">
       <c r="A38" s="6" t="s">
@@ -1892,10 +1901,10 @@
       </c>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
-      <c r="E38" s="19" t="s">
+      <c r="E38" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="F38" s="20">
+      <c r="F38" s="18">
         <f>F36-F37</f>
         <v>0</v>
       </c>
@@ -1909,10 +1918,10 @@
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
-      <c r="E39" s="21" t="s">
+      <c r="E39" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="F39" s="22"/>
+      <c r="F39" s="20"/>
     </row>
     <row r="40" spans="1:6" ht="13.5" thickTop="1">
       <c r="A40" s="8" t="s">
@@ -1923,23 +1932,23 @@
       </c>
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
-      <c r="E40" s="19" t="s">
+      <c r="E40" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="F40" s="20">
+      <c r="F40" s="18">
         <f>F38-F39</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="40" t="s">
+      <c r="A42" s="38" t="s">
         <v>147</v>
       </c>
-      <c r="B42" s="40"/>
-      <c r="C42" s="40"/>
-      <c r="D42" s="40"/>
-      <c r="E42" s="40"/>
-      <c r="F42" s="40"/>
+      <c r="B42" s="38"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="38"/>
+      <c r="F42" s="38"/>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="6" t="s">
@@ -1950,10 +1959,10 @@
       </c>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
-      <c r="E43" s="15" t="s">
+      <c r="E43" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="F43" s="16">
+      <c r="F43" s="14">
         <f>F40</f>
         <v>0</v>
       </c>
@@ -1967,10 +1976,10 @@
       </c>
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
-      <c r="E44" s="15" t="s">
+      <c r="E44" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="F44" s="16"/>
+      <c r="F44" s="14"/>
     </row>
     <row r="45" spans="1:6" ht="13.5" thickBot="1">
       <c r="A45" s="6" t="s">
@@ -1981,10 +1990,10 @@
       </c>
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
-      <c r="E45" s="21" t="s">
+      <c r="E45" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F45" s="22"/>
+      <c r="F45" s="20"/>
     </row>
     <row r="46" spans="1:6" ht="13.5" thickTop="1">
       <c r="A46" s="6" t="s">
@@ -1995,10 +2004,10 @@
       </c>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
-      <c r="E46" s="19" t="s">
+      <c r="E46" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="F46" s="20">
+      <c r="F46" s="18">
         <f>IF(F44 &gt; F45,F44-F45,0)</f>
         <v>0</v>
       </c>
@@ -2012,10 +2021,10 @@
       </c>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
-      <c r="E47" s="21" t="s">
+      <c r="E47" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="F47" s="22"/>
+      <c r="F47" s="20"/>
     </row>
     <row r="48" spans="1:6" ht="13.5" thickTop="1">
       <c r="A48" s="6" t="s">
@@ -2026,10 +2035,10 @@
       </c>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
-      <c r="E48" s="19" t="s">
+      <c r="E48" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="F48" s="20">
+      <c r="F48" s="18">
         <f>F46-F47</f>
         <v>0</v>
       </c>
@@ -2043,10 +2052,10 @@
       </c>
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
-      <c r="E49" s="21" t="s">
+      <c r="E49" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="F49" s="22"/>
+      <c r="F49" s="20"/>
     </row>
     <row r="50" spans="1:6" ht="13.5" thickTop="1">
       <c r="A50" s="6" t="s">
@@ -2057,10 +2066,10 @@
       </c>
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
-      <c r="E50" s="19" t="s">
+      <c r="E50" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="F50" s="20">
+      <c r="F50" s="18">
         <f>IF(F48&gt;F49,F48-F49,0)</f>
         <v>0</v>
       </c>
@@ -2071,7 +2080,7 @@
         <v>90</v>
       </c>
       <c r="C51" s="7"/>
-      <c r="D51" s="32">
+      <c r="D51" s="30">
         <f>F35</f>
         <v>0</v>
       </c>
@@ -2084,7 +2093,7 @@
         <v>91</v>
       </c>
       <c r="C52" s="7"/>
-      <c r="D52" s="32">
+      <c r="D52" s="30">
         <f>D35</f>
         <v>0</v>
       </c>
@@ -2100,10 +2109,10 @@
       </c>
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
-      <c r="E53" s="33" t="s">
+      <c r="E53" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="F53" s="34">
+      <c r="F53" s="32">
         <f>ROUND(IF(D52&lt;&gt;0,D51/D52,0),4)</f>
         <v>0</v>
       </c>
@@ -2117,10 +2126,10 @@
       </c>
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
-      <c r="E54" s="19" t="s">
+      <c r="E54" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="F54" s="20">
+      <c r="F54" s="18">
         <f>ROUND(F50*F53,0)</f>
         <v>0</v>
       </c>
@@ -2134,10 +2143,10 @@
       </c>
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
-      <c r="E55" s="21" t="s">
+      <c r="E55" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="F55" s="22"/>
+      <c r="F55" s="20"/>
     </row>
     <row r="56" spans="1:6" ht="13.5" thickTop="1">
       <c r="A56" s="6" t="s">
@@ -2148,10 +2157,10 @@
       </c>
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
-      <c r="E56" s="19" t="s">
+      <c r="E56" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="F56" s="20">
+      <c r="F56" s="18">
         <f>IF(F54&gt;F55,F54-F55,0)</f>
         <v>0</v>
       </c>
@@ -2165,10 +2174,10 @@
       </c>
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
-      <c r="E57" s="21" t="s">
+      <c r="E57" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="F57" s="22"/>
+      <c r="F57" s="20"/>
     </row>
     <row r="58" spans="1:6" ht="13.5" thickTop="1">
       <c r="A58" s="6" t="s">
@@ -2179,10 +2188,10 @@
       </c>
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
-      <c r="E58" s="19" t="s">
+      <c r="E58" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="F58" s="35">
+      <c r="F58" s="33">
         <f>F56+F57</f>
         <v>0</v>
       </c>
@@ -2194,10 +2203,10 @@
       <c r="B59" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C59" s="15" t="s">
+      <c r="C59" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="D59" s="16"/>
+      <c r="D59" s="14"/>
       <c r="E59" s="7"/>
       <c r="F59" s="11"/>
     </row>
@@ -2208,10 +2217,10 @@
       <c r="B60" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C60" s="21" t="s">
+      <c r="C60" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="D60" s="22"/>
+      <c r="D60" s="20"/>
       <c r="E60" s="7"/>
       <c r="F60" s="11"/>
     </row>
@@ -2222,10 +2231,10 @@
       <c r="B61" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C61" s="19" t="s">
+      <c r="C61" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="D61" s="20">
+      <c r="D61" s="18">
         <f>D59-D60</f>
         <v>0</v>
       </c>
@@ -2239,10 +2248,10 @@
       <c r="B62" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="C62" s="15" t="s">
+      <c r="C62" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="D62" s="16"/>
+      <c r="D62" s="14"/>
       <c r="E62" s="7"/>
       <c r="F62" s="11"/>
     </row>
@@ -2253,10 +2262,10 @@
       <c r="B63" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="C63" s="15" t="s">
+      <c r="C63" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="D63" s="16"/>
+      <c r="D63" s="14"/>
       <c r="E63" s="7"/>
       <c r="F63" s="11"/>
     </row>
@@ -2267,10 +2276,10 @@
       <c r="B64" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="C64" s="15" t="s">
+      <c r="C64" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="D64" s="16"/>
+      <c r="D64" s="14"/>
       <c r="E64" s="7"/>
       <c r="F64" s="11"/>
     </row>
@@ -2281,10 +2290,10 @@
       <c r="B65" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="C65" s="21" t="s">
+      <c r="C65" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="D65" s="22"/>
+      <c r="D65" s="20"/>
       <c r="E65" s="7"/>
       <c r="F65" s="11"/>
     </row>
@@ -2297,10 +2306,10 @@
       </c>
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
-      <c r="E66" s="15" t="s">
+      <c r="E66" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="F66" s="16">
+      <c r="F66" s="14">
         <f>D61+D64+D65</f>
         <v>0</v>
       </c>
@@ -2314,10 +2323,10 @@
       </c>
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
-      <c r="E67" s="15" t="s">
+      <c r="E67" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="F67" s="16"/>
+      <c r="F67" s="14"/>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="6" t="s">
@@ -2328,24 +2337,24 @@
       </c>
       <c r="C68" s="7"/>
       <c r="D68" s="7"/>
-      <c r="E68" s="15" t="s">
+      <c r="E68" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="F68" s="16"/>
+      <c r="F68" s="14"/>
     </row>
     <row r="69" spans="1:6" ht="13.5" thickBot="1">
-      <c r="A69" s="36" t="s">
+      <c r="A69" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="B69" s="37" t="s">
+      <c r="B69" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="C69" s="37"/>
-      <c r="D69" s="37"/>
-      <c r="E69" s="38" t="s">
+      <c r="C69" s="35"/>
+      <c r="D69" s="35"/>
+      <c r="E69" s="36" t="s">
         <v>119</v>
       </c>
-      <c r="F69" s="39">
+      <c r="F69" s="37">
         <f>F58+F66+F67+F68</f>
         <v>0</v>
       </c>
@@ -2359,10 +2368,10 @@
       </c>
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
-      <c r="E70" s="19" t="s">
+      <c r="E70" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="F70" s="20">
+      <c r="F70" s="18">
         <f>F69</f>
         <v>0</v>
       </c>
@@ -2374,223 +2383,237 @@
       <c r="B71" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="C71" s="15" t="s">
+      <c r="C71" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="D71" s="16"/>
+      <c r="D71" s="14"/>
       <c r="E71" s="7"/>
       <c r="F71" s="11"/>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" s="6" t="s">
-        <v>125</v>
+        <v>163</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="C72" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="D72" s="16"/>
+        <v>164</v>
+      </c>
+      <c r="C72" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="D72" s="14"/>
       <c r="E72" s="7"/>
       <c r="F72" s="11"/>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="C73" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="D73" s="16"/>
+        <v>126</v>
+      </c>
+      <c r="C73" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="D73" s="14"/>
       <c r="E73" s="7"/>
       <c r="F73" s="11"/>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="C74" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="D74" s="16"/>
+        <v>159</v>
+      </c>
+      <c r="C74" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="D74" s="14"/>
       <c r="E74" s="7"/>
       <c r="F74" s="11"/>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="C75" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="D75" s="16"/>
+        <v>160</v>
+      </c>
+      <c r="C75" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D75" s="14"/>
       <c r="E75" s="7"/>
       <c r="F75" s="11"/>
     </row>
-    <row r="76" spans="1:6" ht="13.5" thickBot="1">
+    <row r="76" spans="1:6">
       <c r="A76" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="C76" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="D76" s="22"/>
+        <v>161</v>
+      </c>
+      <c r="C76" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="D76" s="14"/>
       <c r="E76" s="7"/>
       <c r="F76" s="11"/>
     </row>
-    <row r="77" spans="1:6" ht="14.25" thickTop="1" thickBot="1">
+    <row r="77" spans="1:6" ht="13.5" thickBot="1">
       <c r="A77" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="C77" s="7"/>
-      <c r="D77" s="7"/>
-      <c r="E77" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="F77" s="22">
-        <f>SUM(D71:D76)</f>
-        <v>0</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="C77" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="D77" s="20"/>
+      <c r="E77" s="7"/>
+      <c r="F77" s="11"/>
     </row>
     <row r="78" spans="1:6" ht="14.25" thickTop="1" thickBot="1">
       <c r="A78" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="C78" s="7"/>
       <c r="D78" s="7"/>
-      <c r="E78" s="21" t="s">
+      <c r="E78" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="F78" s="20">
+        <f>SUM(D71:D77)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="14.25" thickTop="1" thickBot="1">
+      <c r="A79" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="F78" s="22">
-        <f>IF(F77&gt;F70,F77-F70,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="13.5" thickTop="1">
-      <c r="A79" s="6" t="s">
-        <v>135</v>
-      </c>
       <c r="B79" s="7" t="s">
-        <v>157</v>
+        <v>134</v>
       </c>
       <c r="C79" s="7"/>
       <c r="D79" s="7"/>
       <c r="E79" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="F79" s="20">
+        <f>IF(F78&gt;F70,F78-F70,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="13.5" thickTop="1">
+      <c r="A80" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="F79" s="20">
-        <f>F78-D82</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="13.5" thickBot="1">
-      <c r="A80" s="6" t="s">
-        <v>155</v>
-      </c>
       <c r="B80" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C80" s="7"/>
       <c r="D80" s="7"/>
-      <c r="E80" s="21" t="s">
+      <c r="E80" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="F80" s="18">
+        <f>F79-D83</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="13.5" thickBot="1">
+      <c r="A81" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="F80" s="22"/>
-    </row>
-    <row r="81" spans="1:6" ht="13.5" thickTop="1">
-      <c r="A81" s="6" t="s">
-        <v>153</v>
-      </c>
       <c r="B81" s="7" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C81" s="7"/>
       <c r="D81" s="7"/>
       <c r="E81" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="F81" s="20"/>
+    </row>
+    <row r="82" spans="1:6" ht="13.5" thickTop="1">
+      <c r="A82" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="F81" s="20">
-        <f>F79-F80</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6">
-      <c r="A82" s="6" t="s">
-        <v>136</v>
-      </c>
       <c r="B82" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="C82" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="D82" s="16"/>
-      <c r="E82" s="7"/>
-      <c r="F82" s="11"/>
+        <v>154</v>
+      </c>
+      <c r="C82" s="7"/>
+      <c r="D82" s="7"/>
+      <c r="E82" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="F82" s="18">
+        <f>F80-F81</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="C83" s="7"/>
-      <c r="D83" s="7"/>
-      <c r="E83" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="F83" s="16">
-        <f>MAX(F70-F77,0)</f>
-        <v>0</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="C83" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="D83" s="14"/>
+      <c r="E83" s="7"/>
+      <c r="F83" s="11"/>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C84" s="7"/>
+      <c r="D84" s="7"/>
+      <c r="E84" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="F84" s="14">
+        <f>MAX(F70-F78,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B84" s="7" t="s">
+      <c r="B85" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="C84" s="15" t="s">
+      <c r="C85" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="D84" s="16"/>
-      <c r="E84" s="7"/>
-      <c r="F84" s="11"/>
-    </row>
-    <row r="85" spans="1:6">
-      <c r="A85" s="8" t="s">
+      <c r="D85" s="14"/>
+      <c r="E85" s="7"/>
+      <c r="F85" s="11"/>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B85" s="9" t="s">
+      <c r="B86" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="C85" s="15" t="s">
+      <c r="C86" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="D85" s="16"/>
-      <c r="E85" s="9"/>
-      <c r="F85" s="12"/>
+      <c r="D86" s="14"/>
+      <c r="E86" s="9"/>
+      <c r="F86" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>